<commit_message>
Init free ow, ow_ds total price
</commit_message>
<xml_diff>
--- a/tbl/cds_db_0_10.xlsx
+++ b/tbl/cds_db_0_10.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="4920" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="4920" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Base_Parms" sheetId="13" r:id="rId1"/>
@@ -1448,7 +1448,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1664,7 +1664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -5966,10 +5966,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5996,7 +5996,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -6010,7 +6010,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -6024,7 +6024,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -6038,13 +6038,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D5" s="1">
         <v>6</v>
@@ -6052,13 +6052,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D6" s="1">
         <v>6</v>
@@ -6066,13 +6066,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="D7" s="1">
         <v>6</v>
@@ -6080,13 +6080,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="D8" s="1">
         <v>6</v>
@@ -6094,10 +6094,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>500</v>
@@ -6108,10 +6108,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1">
         <v>500</v>
@@ -6122,10 +6122,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1">
         <v>500</v>
@@ -6136,10 +6136,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1">
         <v>500</v>
@@ -6150,13 +6150,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="D13" s="1">
         <v>6</v>
@@ -6164,7 +6164,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
         <v>4</v>
@@ -6178,7 +6178,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1">
         <v>4</v>
@@ -6192,7 +6192,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>4</v>
@@ -6206,13 +6206,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="D17" s="1">
         <v>6</v>
@@ -6220,10 +6220,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1">
         <v>500</v>
@@ -6234,10 +6234,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1">
         <v>500</v>
@@ -6248,10 +6248,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1">
         <v>500</v>
@@ -6262,13 +6262,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="D21" s="1">
         <v>6</v>
@@ -6276,10 +6276,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C22" s="1">
         <v>400</v>
@@ -6290,13 +6290,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="D23" s="1">
         <v>6</v>
@@ -6304,13 +6304,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C24" s="1">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D24" s="1">
         <v>6</v>
@@ -6318,15 +6318,29 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1">
+        <v>200</v>
+      </c>
+      <c r="D25" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="1">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1">
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
         <v>100</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D26" s="1">
         <v>6</v>
       </c>
     </row>

</xml_diff>